<commit_message>
Completed WBS with tasks assigned
</commit_message>
<xml_diff>
--- a/Week 5 - MS Project/homework/HB WBS Durations.xlsx
+++ b/Week 5 - MS Project/homework/HB WBS Durations.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debra\Google Drive\Work\UW\Project 420\Module 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\db345c\Desktop\School\Week 5\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10836"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="133">
   <si>
     <t>Task Name</t>
   </si>
@@ -420,12 +420,15 @@
   </si>
   <si>
     <t>7-11</t>
+  </si>
+  <si>
+    <t>93-94</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -537,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -552,7 +555,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,10 +571,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,23 +668,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -718,23 +703,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -890,17 +858,17 @@
   <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="65" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="65" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>129</v>
       </c>
@@ -908,22 +876,22 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -932,8 +900,8 @@
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <f>A3+1</f>
         <v>2</v>
       </c>
@@ -947,8 +915,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>3</v>
       </c>
@@ -960,8 +928,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -975,8 +943,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -990,8 +958,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1003,8 +971,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1018,8 +986,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1033,8 +1001,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1048,8 +1016,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1063,8 +1031,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1078,8 +1046,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1093,8 +1061,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1106,8 +1074,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1117,12 +1085,12 @@
       <c r="C16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1136,8 +1104,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1147,12 +1115,12 @@
       <c r="C18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1164,8 +1132,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1175,10 +1143,12 @@
       <c r="C20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="D20" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -1188,10 +1158,12 @@
       <c r="C21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="D21" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1201,10 +1173,12 @@
       <c r="C22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="D22" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -1214,10 +1188,12 @@
       <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="D23" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
@@ -1227,10 +1203,12 @@
       <c r="C24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="D24" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -1240,10 +1218,12 @@
       <c r="C25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="D25" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -1253,10 +1233,12 @@
       <c r="C26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="D26" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1266,10 +1248,12 @@
       <c r="C27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="D27" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -1277,10 +1261,12 @@
         <v>34</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="D28" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -1290,10 +1276,12 @@
       <c r="C29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="D29" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -1303,10 +1291,12 @@
       <c r="C30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+      <c r="D30" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -1316,10 +1306,12 @@
       <c r="C31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="D31" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1329,10 +1321,12 @@
       <c r="C32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+      <c r="D32" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="10">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -1342,10 +1336,12 @@
       <c r="C33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+      <c r="D33" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -1355,10 +1351,12 @@
       <c r="C34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+      <c r="D34" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
@@ -1368,10 +1366,12 @@
       <c r="C35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
+      <c r="D35" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
@@ -1381,10 +1381,12 @@
       <c r="C36" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+      <c r="D36" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1394,10 +1396,12 @@
       <c r="C37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="D37" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -1407,10 +1411,12 @@
       <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="D38" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
@@ -1418,10 +1424,12 @@
         <v>46</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="D39" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="10">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
@@ -1431,10 +1439,12 @@
       <c r="C40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+      <c r="D40" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="10">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
@@ -1444,10 +1454,12 @@
       <c r="C41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+      <c r="D41" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="10">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -1457,10 +1469,12 @@
       <c r="C42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="11">
+      <c r="D42" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="10">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -1470,10 +1484,12 @@
       <c r="C43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+      <c r="D43" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="10">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
@@ -1483,10 +1499,12 @@
       <c r="C44" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+      <c r="D44" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="10">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
@@ -1496,10 +1514,12 @@
       <c r="C45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+      <c r="D45" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="10">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
@@ -1509,10 +1529,12 @@
       <c r="C46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="D46" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="10">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
@@ -1520,10 +1542,12 @@
         <v>54</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="11">
+      <c r="D47" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="10">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
@@ -1533,10 +1557,12 @@
       <c r="C48" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="D48" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="10">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -1546,10 +1572,12 @@
       <c r="C49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="D49" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="10">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
@@ -1557,10 +1585,12 @@
         <v>58</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="11">
+      <c r="D50" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="10">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
@@ -1570,10 +1600,12 @@
       <c r="C51" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="11">
+      <c r="D51" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="10">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -1583,10 +1615,12 @@
       <c r="C52" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="11">
+      <c r="D52" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="10">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
@@ -1596,10 +1630,12 @@
       <c r="C53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="11">
+      <c r="D53" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="10">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
@@ -1609,10 +1645,12 @@
       <c r="C54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="11">
+      <c r="D54" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="10">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
@@ -1622,10 +1660,12 @@
       <c r="C55" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="11">
+      <c r="D55" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="10">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
@@ -1635,10 +1675,12 @@
       <c r="C56" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="11">
+      <c r="D56" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="10">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
@@ -1648,10 +1690,12 @@
       <c r="C57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="11">
+      <c r="D57" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="10">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
@@ -1661,10 +1705,12 @@
       <c r="C58" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="11">
+      <c r="D58" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="10">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
@@ -1672,10 +1718,12 @@
         <v>69</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="11">
+      <c r="D59" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="10">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
@@ -1683,10 +1731,12 @@
         <v>70</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="11">
+      <c r="D60" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="10">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
@@ -1696,10 +1746,12 @@
       <c r="C61" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
+      <c r="D61" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="10">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1709,10 +1761,12 @@
       <c r="C62" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="11">
+      <c r="D62" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="10">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
@@ -1722,10 +1776,12 @@
       <c r="C63" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="11">
+      <c r="D63" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="10">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
@@ -1735,10 +1791,12 @@
       <c r="C64" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="11">
+      <c r="D64" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="10">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
@@ -1746,10 +1804,12 @@
         <v>75</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="11">
+      <c r="D65" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="10">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
@@ -1759,10 +1819,12 @@
       <c r="C66" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="11">
+      <c r="D66" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="10">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
@@ -1772,10 +1834,12 @@
       <c r="C67" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="11">
+      <c r="D67" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="10">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
@@ -1785,10 +1849,12 @@
       <c r="C68" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="11">
+      <c r="D68" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="10">
         <f t="shared" ref="A69:A113" si="1">A68+1</f>
         <v>67</v>
       </c>
@@ -1798,10 +1864,12 @@
       <c r="C69" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="11">
+      <c r="D69" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="10">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
@@ -1811,10 +1879,12 @@
       <c r="C70" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="11">
+      <c r="D70" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="10">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
@@ -1824,10 +1894,12 @@
       <c r="C71" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="11">
+      <c r="D71" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="10">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
@@ -1835,10 +1907,12 @@
         <v>82</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="11">
+      <c r="D72" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="10">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
@@ -1848,10 +1922,12 @@
       <c r="C73" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="11">
+      <c r="D73" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="10">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
@@ -1861,10 +1937,12 @@
       <c r="C74" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="11">
+      <c r="D74" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="10">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -1874,10 +1952,12 @@
       <c r="C75" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="11">
+      <c r="D75" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="10">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
@@ -1887,10 +1967,12 @@
       <c r="C76" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D76" s="3"/>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="11">
+      <c r="D76" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="10">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
@@ -1900,10 +1982,12 @@
       <c r="C77" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D77" s="3"/>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="11">
+      <c r="D77" s="3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="10">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
@@ -1913,10 +1997,12 @@
       <c r="C78" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D78" s="3"/>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="11">
+      <c r="D78" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="10">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
@@ -1924,10 +2010,12 @@
         <v>89</v>
       </c>
       <c r="C79" s="1"/>
-      <c r="D79" s="3"/>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="11">
+      <c r="D79" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="10">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
@@ -1937,10 +2025,12 @@
       <c r="C80" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="11">
+      <c r="D80" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="10">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
@@ -1950,10 +2040,12 @@
       <c r="C81" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D81" s="3"/>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="11">
+      <c r="D81" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="10">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
@@ -1963,10 +2055,12 @@
       <c r="C82" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D82" s="3"/>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="11">
+      <c r="D82" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="10">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
@@ -1976,10 +2070,12 @@
       <c r="C83" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="11">
+      <c r="D83" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="10">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
@@ -1987,10 +2083,12 @@
         <v>94</v>
       </c>
       <c r="C84" s="1"/>
-      <c r="D84" s="3"/>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="11">
+      <c r="D84" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="10">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
@@ -2000,10 +2098,12 @@
       <c r="C85" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D85" s="3"/>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="11">
+      <c r="D85" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="10">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
@@ -2013,10 +2113,12 @@
       <c r="C86" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D86" s="3"/>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="11">
+      <c r="D86" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="10">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
@@ -2026,10 +2128,12 @@
       <c r="C87" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="11">
+      <c r="D87" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="10">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
@@ -2039,10 +2143,12 @@
       <c r="C88" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="11">
+      <c r="D88" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="10">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
@@ -2050,10 +2156,12 @@
         <v>99</v>
       </c>
       <c r="C89" s="1"/>
-      <c r="D89" s="3"/>
-    </row>
-    <row r="90" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="11">
+      <c r="D89" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="10">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -2063,10 +2171,12 @@
       <c r="C90" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="11">
+      <c r="D90" s="3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="10">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
@@ -2076,10 +2186,12 @@
       <c r="C91" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D91" s="3"/>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="11">
+      <c r="D91" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="10">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
@@ -2089,10 +2201,12 @@
       <c r="C92" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D92" s="3"/>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="11">
+      <c r="D92" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="10">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
@@ -2102,10 +2216,12 @@
       <c r="C93" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D93" s="3"/>
-    </row>
-    <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="11">
+      <c r="D93" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="10">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -2113,10 +2229,12 @@
         <v>104</v>
       </c>
       <c r="C94" s="1"/>
-      <c r="D94" s="3"/>
-    </row>
-    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="11">
+      <c r="D94" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="10">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
@@ -2126,10 +2244,12 @@
       <c r="C95" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D95" s="3"/>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="11">
+      <c r="D95" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="10">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
@@ -2139,10 +2259,12 @@
       <c r="C96" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D96" s="3"/>
-    </row>
-    <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="11">
+      <c r="D96" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="10">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
@@ -2152,10 +2274,12 @@
       <c r="C97" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="11">
+      <c r="D97" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="10">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
@@ -2163,10 +2287,12 @@
         <v>108</v>
       </c>
       <c r="C98" s="1"/>
-      <c r="D98" s="3"/>
-    </row>
-    <row r="99" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="11">
+      <c r="D98" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="10">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
@@ -2176,10 +2302,12 @@
       <c r="C99" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D99" s="3"/>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="11">
+      <c r="D99" s="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="10">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
@@ -2189,10 +2317,12 @@
       <c r="C100" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D100" s="3"/>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="11">
+      <c r="D100" s="3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="10">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
@@ -2202,10 +2332,12 @@
       <c r="C101" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D101" s="3"/>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="11">
+      <c r="D101" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="10">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -2215,10 +2347,12 @@
       <c r="C102" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D102" s="3"/>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="11">
+      <c r="D102" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="10">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -2226,10 +2360,12 @@
         <v>113</v>
       </c>
       <c r="C103" s="1"/>
-      <c r="D103" s="3"/>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="11">
+      <c r="D103" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="10">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
@@ -2239,10 +2375,12 @@
       <c r="C104" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D104" s="3"/>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="11">
+      <c r="D104" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="10">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
@@ -2252,10 +2390,12 @@
       <c r="C105" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D105" s="3"/>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="11">
+      <c r="D105" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="10">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
@@ -2265,10 +2405,12 @@
       <c r="C106" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D106" s="3"/>
-    </row>
-    <row r="107" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="11">
+      <c r="D106" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="10">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
@@ -2278,10 +2420,12 @@
       <c r="C107" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D107" s="3"/>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="11">
+      <c r="D107" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="10">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
@@ -2289,10 +2433,12 @@
         <v>118</v>
       </c>
       <c r="C108" s="1"/>
-      <c r="D108" s="3"/>
-    </row>
-    <row r="109" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="11">
+      <c r="D108" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="10">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
@@ -2302,10 +2448,12 @@
       <c r="C109" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D109" s="3"/>
-    </row>
-    <row r="110" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="11">
+      <c r="D109" s="3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="10">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
@@ -2315,10 +2463,12 @@
       <c r="C110" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D110" s="3"/>
-    </row>
-    <row r="111" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="11">
+      <c r="D110" s="3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="10">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
@@ -2328,10 +2478,12 @@
       <c r="C111" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D111" s="3"/>
-    </row>
-    <row r="112" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="11">
+      <c r="D111" s="3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="10">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
@@ -2341,10 +2493,12 @@
       <c r="C112" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D112" s="3"/>
-    </row>
-    <row r="113" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="11">
+      <c r="D112" s="3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="10">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
@@ -2354,7 +2508,9 @@
       <c r="C113" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D113" s="6"/>
+      <c r="D113" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>